<commit_message>
avoid index column in spreadsheet by using custom writer
</commit_message>
<xml_diff>
--- a/scripts/spreadsheet_handling/out.xlsx
+++ b/scripts/spreadsheet_handling/out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>kunde</t>
   </si>
@@ -84,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -92,30 +92,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,78 +396,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="C2:D2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>